<commit_message>
Site updated: 2025-08-07 23:51:37
</commit_message>
<xml_diff>
--- a/travel-map/截至20250806.xlsx
+++ b/travel-map/截至20250806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myblog\source\travel-map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F106F61-F736-451B-B1BE-AD0B3E00376D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14323591-10B2-48E8-B999-483513E08524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="134">
   <si>
     <t>time</t>
   </si>
@@ -196,15 +196,6 @@
     <t>兴安盟</t>
   </si>
   <si>
-    <t>四平市</t>
-  </si>
-  <si>
-    <t>松原市</t>
-  </si>
-  <si>
-    <t>朔州市</t>
-  </si>
-  <si>
     <t>晋中市</t>
   </si>
   <si>
@@ -304,9 +295,6 @@
     <t>阿拉善盟</t>
   </si>
   <si>
-    <t>白银市</t>
-  </si>
-  <si>
     <t>兰州市</t>
   </si>
   <si>
@@ -316,9 +304,6 @@
     <t>乌海市</t>
   </si>
   <si>
-    <t>吴忠市</t>
-  </si>
-  <si>
     <t>宁夏回族自治区</t>
   </si>
   <si>
@@ -349,21 +334,12 @@
     <t>海东市</t>
   </si>
   <si>
-    <t>可克达拉市</t>
-  </si>
-  <si>
     <t>乐山市</t>
   </si>
   <si>
     <t>南京市</t>
   </si>
   <si>
-    <t>石河子市</t>
-  </si>
-  <si>
-    <t>塔城地区</t>
-  </si>
-  <si>
     <t>五家渠市</t>
   </si>
   <si>
@@ -416,9 +392,6 @@
   </si>
   <si>
     <t>牡丹江市</t>
-  </si>
-  <si>
-    <t>沈阳市</t>
   </si>
   <si>
     <t>延边朝鲜族自治州</t>
@@ -436,6 +409,26 @@
   </si>
   <si>
     <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>常住</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>广东省</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>沈阳市</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>辽宁省</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>石河子市</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -504,11 +497,12 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="STYLE0" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -812,25 +806,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.19921875" customWidth="1"/>
     <col min="2" max="2" width="16.9296875" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -844,206 +839,206 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" t="s">
-        <v>137</v>
+        <v>75</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45444</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
-        <v>137</v>
+      <c r="C4" s="2">
+        <v>45108</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>137</v>
+      <c r="C5" s="2">
+        <v>45108</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" t="s">
-        <v>137</v>
+        <v>84</v>
+      </c>
+      <c r="C6" s="2">
+        <v>45383</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" t="s">
-        <v>137</v>
+        <v>84</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45383</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" t="s">
-        <v>137</v>
+        <v>84</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45352</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" t="s">
-        <v>137</v>
+        <v>84</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45352</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" t="s">
-        <v>137</v>
+        <v>84</v>
+      </c>
+      <c r="C10" s="2">
+        <v>45383</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E10" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" t="s">
-        <v>137</v>
+        <v>13</v>
+      </c>
+      <c r="C11" s="2">
+        <v>45474</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>137</v>
+      <c r="C12" s="2">
+        <v>45474</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
-        <v>137</v>
+      <c r="C13" s="2">
+        <v>45748</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1053,405 +1048,405 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
-        <v>137</v>
+      <c r="C14" s="2">
+        <v>45748</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
-        <v>137</v>
+      <c r="C15" s="2">
+        <v>45474</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E15" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>137</v>
+        <v>130</v>
+      </c>
+      <c r="C16" s="2">
+        <v>45444</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>137</v>
+        <v>28</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45689</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E17" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
-        <v>137</v>
+      <c r="C18" s="2">
+        <v>44927</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E18" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
-        <v>137</v>
+      <c r="C19" s="2">
+        <v>45689</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="s">
-        <v>137</v>
+      <c r="C20" s="2">
+        <v>45689</v>
       </c>
       <c r="D20" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E20" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
-        <v>137</v>
+      <c r="C21" s="2">
+        <v>44958</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E21" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
-        <v>137</v>
+      <c r="C22" s="2">
+        <v>45689</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="s">
-        <v>137</v>
+        <v>43</v>
+      </c>
+      <c r="C23" s="2">
+        <v>45597</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E23" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" t="s">
-        <v>137</v>
+      <c r="C24" s="2">
+        <v>45474</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E24" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
       </c>
-      <c r="C25" t="s">
-        <v>137</v>
+      <c r="C25" s="2">
+        <v>45292</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="C26" t="s">
-        <v>137</v>
+      <c r="C26" s="2">
+        <v>45170</v>
       </c>
       <c r="D26" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
-        <v>137</v>
+        <v>17</v>
+      </c>
+      <c r="C27" s="2">
+        <v>45292</v>
       </c>
       <c r="D27" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
       </c>
-      <c r="C28" t="s">
-        <v>137</v>
+      <c r="C28" s="2">
+        <v>45108</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E28" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
       </c>
-      <c r="C29" t="s">
-        <v>137</v>
+      <c r="C29" s="2">
+        <v>45689</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E29" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>137</v>
+        <v>23</v>
+      </c>
+      <c r="C30" s="2">
+        <v>45566</v>
       </c>
       <c r="D30" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E30" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>23</v>
       </c>
-      <c r="C31" t="s">
-        <v>137</v>
+      <c r="C31" s="2">
+        <v>45200</v>
       </c>
       <c r="D31" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E31" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
       </c>
-      <c r="C32" t="s">
-        <v>137</v>
+      <c r="C32" s="2">
+        <v>45200</v>
       </c>
       <c r="D32" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
       </c>
-      <c r="C33" t="s">
-        <v>137</v>
+      <c r="C33" s="2">
+        <v>45200</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E33" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
       </c>
-      <c r="C34" t="s">
-        <v>137</v>
+      <c r="C34" s="2">
+        <v>45658</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E34" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
       </c>
-      <c r="C35" t="s">
-        <v>137</v>
+      <c r="C35" s="2">
+        <v>45658</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
         <v>23</v>
       </c>
-      <c r="C36" t="s">
-        <v>137</v>
+      <c r="C36" s="2">
+        <v>45566</v>
       </c>
       <c r="D36" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E36" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" t="s">
-        <v>137</v>
+        <v>33</v>
+      </c>
+      <c r="C37" s="2">
+        <v>45108</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1461,1243 +1456,1124 @@
       <c r="B38" t="s">
         <v>33</v>
       </c>
-      <c r="C38" t="s">
-        <v>137</v>
+      <c r="C38" s="2">
+        <v>45108</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" t="s">
-        <v>137</v>
+        <v>47</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45108</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E39" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" t="s">
-        <v>137</v>
+        <v>45</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45658</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E40" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="B41" t="s">
         <v>45</v>
       </c>
-      <c r="C41" t="s">
-        <v>137</v>
+      <c r="C41" s="2">
+        <v>45658</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E41" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" t="s">
-        <v>137</v>
+      <c r="C42" s="2">
+        <v>45200</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E42" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" t="s">
-        <v>137</v>
+        <v>8</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45292</v>
       </c>
       <c r="D43" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E43" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" t="s">
-        <v>137</v>
+        <v>8</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45809</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E44" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" t="s">
-        <v>137</v>
+        <v>35</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45017</v>
       </c>
       <c r="D45" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E45" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" t="s">
-        <v>137</v>
+        <v>51</v>
+      </c>
+      <c r="C46" s="2">
+        <v>45566</v>
       </c>
       <c r="D46" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E46" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" t="s">
-        <v>137</v>
+        <v>51</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45566</v>
       </c>
       <c r="D47" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E47" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" t="s">
-        <v>137</v>
+        <v>132</v>
+      </c>
+      <c r="C48" s="2">
+        <v>45658</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E48" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" t="s">
-        <v>137</v>
+        <v>10</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45352</v>
       </c>
       <c r="D49" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E49" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" t="s">
-        <v>137</v>
+        <v>10</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45017</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E50" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" t="s">
-        <v>137</v>
+        <v>10</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45139</v>
       </c>
       <c r="D51" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E51" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
       </c>
-      <c r="C52" t="s">
-        <v>137</v>
+      <c r="C52" s="2">
+        <v>45689</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E52" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
       </c>
-      <c r="C53" t="s">
-        <v>137</v>
+      <c r="C53" s="2">
+        <v>45536</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E53" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
       </c>
-      <c r="C54" t="s">
-        <v>137</v>
+      <c r="C54" s="2">
+        <v>45200</v>
       </c>
       <c r="D54" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E54" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
       </c>
-      <c r="C55" t="s">
-        <v>137</v>
+      <c r="C55" s="2">
+        <v>45566</v>
       </c>
       <c r="D55" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E55" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
       </c>
-      <c r="C56" t="s">
-        <v>137</v>
+      <c r="C56" s="2">
+        <v>45352</v>
       </c>
       <c r="D56" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E56" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
       </c>
-      <c r="C57" t="s">
-        <v>137</v>
+      <c r="C57" s="2">
+        <v>45078</v>
       </c>
       <c r="D57" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E57" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C58" t="s">
-        <v>137</v>
+      <c r="C58" s="2">
+        <v>45474</v>
       </c>
       <c r="D58" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E58" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
       </c>
-      <c r="C59" t="s">
-        <v>137</v>
+      <c r="C59" s="2">
+        <v>45566</v>
       </c>
       <c r="D59" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E59" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" t="s">
-        <v>137</v>
+        <v>94</v>
+      </c>
+      <c r="C60" s="2">
+        <v>45352</v>
       </c>
       <c r="D60" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E60" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" t="s">
-        <v>137</v>
+        <v>94</v>
+      </c>
+      <c r="C61" s="2">
+        <v>45352</v>
       </c>
       <c r="D61" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E61" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" t="s">
-        <v>137</v>
+        <v>82</v>
+      </c>
+      <c r="C62" s="2">
+        <v>45383</v>
       </c>
       <c r="D62" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E62" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>99</v>
-      </c>
-      <c r="C63" t="s">
-        <v>137</v>
+        <v>82</v>
+      </c>
+      <c r="C63" s="2">
+        <v>45292</v>
       </c>
       <c r="D63" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E63" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
-      </c>
-      <c r="C64" t="s">
-        <v>137</v>
+        <v>82</v>
+      </c>
+      <c r="C64" s="2">
+        <v>45292</v>
       </c>
       <c r="D64" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E64" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
-      </c>
-      <c r="C65" t="s">
-        <v>137</v>
+        <v>37</v>
+      </c>
+      <c r="C65" s="2">
+        <v>45078</v>
       </c>
       <c r="D65" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E65" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
-      </c>
-      <c r="C66" t="s">
-        <v>137</v>
+        <v>37</v>
+      </c>
+      <c r="C66" s="2">
+        <v>45078</v>
       </c>
       <c r="D66" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
-      </c>
-      <c r="C67" t="s">
-        <v>137</v>
+        <v>21</v>
+      </c>
+      <c r="C67" s="2">
+        <v>45170</v>
       </c>
       <c r="D67" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E67" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
-      </c>
-      <c r="C68" t="s">
-        <v>137</v>
+        <v>21</v>
+      </c>
+      <c r="C68" s="2">
+        <v>45505</v>
       </c>
       <c r="D68" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E68" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
-      </c>
-      <c r="C69" t="s">
-        <v>137</v>
+        <v>21</v>
+      </c>
+      <c r="C69" s="2">
+        <v>45292</v>
       </c>
       <c r="D69" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E69" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>37</v>
-      </c>
-      <c r="C70" t="s">
-        <v>137</v>
+        <v>21</v>
+      </c>
+      <c r="C70" s="2">
+        <v>45505</v>
       </c>
       <c r="D70" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E70" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="B71" t="s">
         <v>21</v>
       </c>
-      <c r="C71" t="s">
-        <v>137</v>
+      <c r="C71" s="2">
+        <v>45505</v>
       </c>
       <c r="D71" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E71" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
         <v>21</v>
       </c>
-      <c r="C72" t="s">
-        <v>137</v>
+      <c r="C72" s="2">
+        <v>45292</v>
       </c>
       <c r="D72" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E72" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
-      </c>
-      <c r="C73" t="s">
-        <v>137</v>
+        <v>74</v>
+      </c>
+      <c r="C73" s="2">
+        <v>45474</v>
       </c>
       <c r="D73" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E73" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="B74" t="s">
-        <v>21</v>
-      </c>
-      <c r="C74" t="s">
-        <v>137</v>
+        <v>6</v>
+      </c>
+      <c r="C74" s="2">
+        <v>45108</v>
       </c>
       <c r="D74" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E74" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B75" t="s">
-        <v>21</v>
-      </c>
-      <c r="C75" t="s">
-        <v>137</v>
+        <v>65</v>
+      </c>
+      <c r="C75" s="2">
+        <v>45717</v>
       </c>
       <c r="D75" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E75" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>21</v>
-      </c>
-      <c r="C76" t="s">
-        <v>137</v>
+        <v>65</v>
+      </c>
+      <c r="C76" s="2">
+        <v>45292</v>
       </c>
       <c r="D76" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E76" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>21</v>
-      </c>
-      <c r="C77" t="s">
-        <v>137</v>
+        <v>65</v>
+      </c>
+      <c r="C77" s="2">
+        <v>45474</v>
       </c>
       <c r="D77" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E77" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" t="s">
-        <v>137</v>
+        <v>65</v>
+      </c>
+      <c r="C78" s="2">
+        <v>45292</v>
       </c>
       <c r="D78" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E78" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" t="s">
-        <v>137</v>
+        <v>65</v>
+      </c>
+      <c r="C79" s="2">
+        <v>45474</v>
       </c>
       <c r="D79" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E79" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
-      </c>
-      <c r="C80" t="s">
-        <v>137</v>
+        <v>39</v>
+      </c>
+      <c r="C80" s="2">
+        <v>44896</v>
       </c>
       <c r="D80" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E80" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="B81" t="s">
-        <v>68</v>
-      </c>
-      <c r="C81" t="s">
-        <v>137</v>
+        <v>63</v>
+      </c>
+      <c r="C81" s="2">
+        <v>45474</v>
       </c>
       <c r="D81" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E81" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B82" t="s">
-        <v>68</v>
-      </c>
-      <c r="C82" t="s">
-        <v>137</v>
+        <v>63</v>
+      </c>
+      <c r="C82" s="2">
+        <v>45474</v>
       </c>
       <c r="D82" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E82" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B83" t="s">
-        <v>68</v>
-      </c>
-      <c r="C83" t="s">
-        <v>137</v>
+        <v>63</v>
+      </c>
+      <c r="C83" s="2">
+        <v>45474</v>
       </c>
       <c r="D83" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E83" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
-      </c>
-      <c r="C84" t="s">
-        <v>137</v>
+        <v>63</v>
+      </c>
+      <c r="C84" s="2">
+        <v>45505</v>
       </c>
       <c r="D84" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E84" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="B85" t="s">
-        <v>39</v>
-      </c>
-      <c r="C85" t="s">
-        <v>137</v>
+        <v>63</v>
+      </c>
+      <c r="C85" s="2">
+        <v>45505</v>
       </c>
       <c r="D85" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E85" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
-      </c>
-      <c r="C86" t="s">
-        <v>137</v>
+        <v>63</v>
+      </c>
+      <c r="C86" s="2">
+        <v>45505</v>
       </c>
       <c r="D86" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E86" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="B87" t="s">
-        <v>66</v>
-      </c>
-      <c r="C87" t="s">
-        <v>137</v>
+        <v>15</v>
+      </c>
+      <c r="C87" s="2">
+        <v>45748</v>
       </c>
       <c r="D87" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E87" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B88" t="s">
-        <v>66</v>
-      </c>
-      <c r="C88" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C88" s="2">
+        <v>45689</v>
       </c>
       <c r="D88" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E88" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="B89" t="s">
-        <v>66</v>
-      </c>
-      <c r="C89" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C89" s="2">
+        <v>45689</v>
       </c>
       <c r="D89" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E89" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B90" t="s">
-        <v>66</v>
-      </c>
-      <c r="C90" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C90" s="2">
+        <v>45292</v>
       </c>
       <c r="D90" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E90" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="B91" t="s">
-        <v>66</v>
-      </c>
-      <c r="C91" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C91" s="2">
+        <v>45292</v>
       </c>
       <c r="D91" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E91" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B92" t="s">
-        <v>15</v>
-      </c>
-      <c r="C92" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C92" s="2">
+        <v>45383</v>
       </c>
       <c r="D92" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E92" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B93" t="s">
-        <v>83</v>
-      </c>
-      <c r="C93" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C93" s="2">
+        <v>45689</v>
       </c>
       <c r="D93" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E93" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B94" t="s">
-        <v>83</v>
-      </c>
-      <c r="C94" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C94" s="2">
+        <v>45689</v>
       </c>
       <c r="D94" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E94" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B95" t="s">
-        <v>83</v>
-      </c>
-      <c r="C95" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C95" s="2">
+        <v>45689</v>
       </c>
       <c r="D95" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E95" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B96" t="s">
-        <v>83</v>
-      </c>
-      <c r="C96" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C96" s="2">
+        <v>45689</v>
       </c>
       <c r="D96" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E96" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
-      </c>
-      <c r="C97" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C97" s="2">
+        <v>45292</v>
       </c>
       <c r="D97" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E97" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
-      </c>
-      <c r="C98" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C98" s="2">
+        <v>45383</v>
       </c>
       <c r="D98" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E98" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="B99" t="s">
-        <v>83</v>
-      </c>
-      <c r="C99" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C99" s="2">
+        <v>45292</v>
       </c>
       <c r="D99" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E99" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B100" t="s">
-        <v>83</v>
-      </c>
-      <c r="C100" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C100" s="2">
+        <v>45292</v>
       </c>
       <c r="D100" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E100" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B101" t="s">
-        <v>83</v>
-      </c>
-      <c r="C101" t="s">
-        <v>137</v>
+        <v>80</v>
+      </c>
+      <c r="C101" s="2">
+        <v>45292</v>
       </c>
       <c r="D101" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E101" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>125</v>
+        <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>83</v>
-      </c>
-      <c r="C102" t="s">
-        <v>137</v>
+        <v>4</v>
+      </c>
+      <c r="C102" s="2">
+        <v>45839</v>
       </c>
       <c r="D102" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E102" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="B103" t="s">
-        <v>83</v>
-      </c>
-      <c r="C103" t="s">
-        <v>137</v>
+        <v>4</v>
+      </c>
+      <c r="C103" s="2">
+        <v>45839</v>
       </c>
       <c r="D103" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E103" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>82</v>
-      </c>
-      <c r="B104" t="s">
-        <v>83</v>
-      </c>
-      <c r="C104" t="s">
-        <v>137</v>
-      </c>
-      <c r="D104" t="s">
-        <v>137</v>
-      </c>
-      <c r="E104" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>107</v>
-      </c>
-      <c r="B105" t="s">
-        <v>83</v>
-      </c>
-      <c r="C105" t="s">
-        <v>137</v>
-      </c>
-      <c r="D105" t="s">
-        <v>137</v>
-      </c>
-      <c r="E105" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>106</v>
-      </c>
-      <c r="B106" t="s">
-        <v>83</v>
-      </c>
-      <c r="C106" t="s">
-        <v>137</v>
-      </c>
-      <c r="D106" t="s">
-        <v>137</v>
-      </c>
-      <c r="E106" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>122</v>
-      </c>
-      <c r="B107" t="s">
-        <v>83</v>
-      </c>
-      <c r="C107" t="s">
-        <v>137</v>
-      </c>
-      <c r="D107" t="s">
-        <v>137</v>
-      </c>
-      <c r="E107" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>121</v>
-      </c>
-      <c r="B108" t="s">
-        <v>83</v>
-      </c>
-      <c r="C108" t="s">
-        <v>137</v>
-      </c>
-      <c r="D108" t="s">
-        <v>137</v>
-      </c>
-      <c r="E108" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>5</v>
-      </c>
-      <c r="B109" t="s">
-        <v>4</v>
-      </c>
-      <c r="C109" t="s">
-        <v>137</v>
-      </c>
-      <c r="D109" t="s">
-        <v>137</v>
-      </c>
-      <c r="E109" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>3</v>
-      </c>
-      <c r="B110" t="s">
-        <v>4</v>
-      </c>
-      <c r="C110" t="s">
-        <v>137</v>
-      </c>
-      <c r="D110" t="s">
-        <v>137</v>
-      </c>
-      <c r="E110" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E110">
-    <sortCondition ref="B14:B110"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E112">
+    <sortCondition ref="B1:B112"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Site updated: 2025-08-08 00:03:15
</commit_message>
<xml_diff>
--- a/travel-map/截至20250806.xlsx
+++ b/travel-map/截至20250806.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myblog\source\travel-map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14323591-10B2-48E8-B999-483513E08524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7596FE42-3977-4525-96F6-AB415310C603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="截至20250806.shp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="158">
   <si>
     <t>time</t>
   </si>
@@ -412,10 +423,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>常住</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>广东省</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -430,6 +437,81 @@
   <si>
     <t>石河子市</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024年6月</t>
+  </si>
+  <si>
+    <t>常住</t>
+  </si>
+  <si>
+    <t>2023年7月</t>
+  </si>
+  <si>
+    <t>2024年4月</t>
+  </si>
+  <si>
+    <t>2024年3月</t>
+  </si>
+  <si>
+    <t>2024年7月</t>
+  </si>
+  <si>
+    <t>2025年4月</t>
+  </si>
+  <si>
+    <t>2025年2月</t>
+  </si>
+  <si>
+    <t>2023年1月</t>
+  </si>
+  <si>
+    <t>2023年2月</t>
+  </si>
+  <si>
+    <t>2024年11月</t>
+  </si>
+  <si>
+    <t>2024年1月</t>
+  </si>
+  <si>
+    <t>2023年9月</t>
+  </si>
+  <si>
+    <t>2024年10月</t>
+  </si>
+  <si>
+    <t>2023年10月</t>
+  </si>
+  <si>
+    <t>2025年1月</t>
+  </si>
+  <si>
+    <t>2025年6月</t>
+  </si>
+  <si>
+    <t>2023年4月</t>
+  </si>
+  <si>
+    <t>2023年8月</t>
+  </si>
+  <si>
+    <t>2024年9月</t>
+  </si>
+  <si>
+    <t>2023年6月</t>
+  </si>
+  <si>
+    <t>2024年8月</t>
+  </si>
+  <si>
+    <t>2025年3月</t>
+  </si>
+  <si>
+    <t>2022年12月</t>
+  </si>
+  <si>
+    <t>2025年7月</t>
   </si>
 </sst>
 </file>
@@ -808,15 +890,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.19921875" customWidth="1"/>
     <col min="2" max="2" width="16.9296875" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -844,8 +926,8 @@
       <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="2">
-        <v>45444</v>
+      <c r="C2" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="D2" t="s">
         <v>128</v>
@@ -862,7 +944,7 @@
         <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
         <v>128</v>
@@ -878,8 +960,8 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2">
-        <v>45108</v>
+      <c r="C4" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D4" t="s">
         <v>128</v>
@@ -895,8 +977,8 @@
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2">
-        <v>45108</v>
+      <c r="C5" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D5" t="s">
         <v>128</v>
@@ -912,8 +994,8 @@
       <c r="B6" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="2">
-        <v>45383</v>
+      <c r="C6" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D6" t="s">
         <v>128</v>
@@ -929,8 +1011,8 @@
       <c r="B7" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="2">
-        <v>45383</v>
+      <c r="C7" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D7" t="s">
         <v>128</v>
@@ -946,8 +1028,8 @@
       <c r="B8" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="2">
-        <v>45352</v>
+      <c r="C8" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="D8" t="s">
         <v>128</v>
@@ -963,8 +1045,8 @@
       <c r="B9" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="2">
-        <v>45352</v>
+      <c r="C9" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="D9" t="s">
         <v>128</v>
@@ -980,8 +1062,8 @@
       <c r="B10" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="2">
-        <v>45383</v>
+      <c r="C10" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D10" t="s">
         <v>128</v>
@@ -997,8 +1079,8 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2">
-        <v>45474</v>
+      <c r="C11" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D11" t="s">
         <v>128</v>
@@ -1014,8 +1096,8 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2">
-        <v>45474</v>
+      <c r="C12" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D12" t="s">
         <v>128</v>
@@ -1031,8 +1113,8 @@
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2">
-        <v>45748</v>
+      <c r="C13" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="D13" t="s">
         <v>128</v>
@@ -1048,8 +1130,8 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2">
-        <v>45748</v>
+      <c r="C14" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="D14" t="s">
         <v>128</v>
@@ -1065,8 +1147,8 @@
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2">
-        <v>45474</v>
+      <c r="C15" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D15" t="s">
         <v>128</v>
@@ -1080,10 +1162,10 @@
         <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="2">
-        <v>45444</v>
+        <v>129</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="D16" t="s">
         <v>128</v>
@@ -1099,8 +1181,8 @@
       <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="2">
-        <v>45689</v>
+      <c r="C17" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D17" t="s">
         <v>128</v>
@@ -1116,8 +1198,8 @@
       <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="2">
-        <v>44927</v>
+      <c r="C18" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="D18" t="s">
         <v>128</v>
@@ -1133,8 +1215,8 @@
       <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="2">
-        <v>45689</v>
+      <c r="C19" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D19" t="s">
         <v>128</v>
@@ -1150,8 +1232,8 @@
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="2">
-        <v>45689</v>
+      <c r="C20" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D20" t="s">
         <v>128</v>
@@ -1167,8 +1249,8 @@
       <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2">
-        <v>44958</v>
+      <c r="C21" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="D21" t="s">
         <v>128</v>
@@ -1184,8 +1266,8 @@
       <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="2">
-        <v>45689</v>
+      <c r="C22" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D22" t="s">
         <v>128</v>
@@ -1201,8 +1283,8 @@
       <c r="B23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="2">
-        <v>45597</v>
+      <c r="C23" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="D23" t="s">
         <v>128</v>
@@ -1218,8 +1300,8 @@
       <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="2">
-        <v>45474</v>
+      <c r="C24" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D24" t="s">
         <v>128</v>
@@ -1235,8 +1317,8 @@
       <c r="B25" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="2">
-        <v>45292</v>
+      <c r="C25" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D25" t="s">
         <v>128</v>
@@ -1252,8 +1334,8 @@
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="2">
-        <v>45170</v>
+      <c r="C26" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="D26" t="s">
         <v>128</v>
@@ -1269,8 +1351,8 @@
       <c r="B27" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="2">
-        <v>45292</v>
+      <c r="C27" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D27" t="s">
         <v>128</v>
@@ -1286,8 +1368,8 @@
       <c r="B28" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="2">
-        <v>45108</v>
+      <c r="C28" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D28" t="s">
         <v>128</v>
@@ -1303,8 +1385,8 @@
       <c r="B29" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="2">
-        <v>45689</v>
+      <c r="C29" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D29" t="s">
         <v>128</v>
@@ -1320,8 +1402,8 @@
       <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="2">
-        <v>45566</v>
+      <c r="C30" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D30" t="s">
         <v>128</v>
@@ -1337,8 +1419,8 @@
       <c r="B31" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="2">
-        <v>45200</v>
+      <c r="C31" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="D31" t="s">
         <v>128</v>
@@ -1354,8 +1436,8 @@
       <c r="B32" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="2">
-        <v>45200</v>
+      <c r="C32" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="D32" t="s">
         <v>128</v>
@@ -1371,8 +1453,8 @@
       <c r="B33" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="2">
-        <v>45200</v>
+      <c r="C33" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="D33" t="s">
         <v>128</v>
@@ -1388,8 +1470,8 @@
       <c r="B34" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="2">
-        <v>45658</v>
+      <c r="C34" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D34" t="s">
         <v>128</v>
@@ -1405,8 +1487,8 @@
       <c r="B35" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="2">
-        <v>45658</v>
+      <c r="C35" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D35" t="s">
         <v>128</v>
@@ -1422,8 +1504,8 @@
       <c r="B36" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="2">
-        <v>45566</v>
+      <c r="C36" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D36" t="s">
         <v>128</v>
@@ -1439,8 +1521,8 @@
       <c r="B37" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="2">
-        <v>45108</v>
+      <c r="C37" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D37" t="s">
         <v>128</v>
@@ -1456,8 +1538,8 @@
       <c r="B38" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="2">
-        <v>45108</v>
+      <c r="C38" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D38" t="s">
         <v>128</v>
@@ -1473,8 +1555,8 @@
       <c r="B39" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="2">
-        <v>45108</v>
+      <c r="C39" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D39" t="s">
         <v>128</v>
@@ -1490,8 +1572,8 @@
       <c r="B40" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="2">
-        <v>45658</v>
+      <c r="C40" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D40" t="s">
         <v>128</v>
@@ -1507,8 +1589,8 @@
       <c r="B41" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="2">
-        <v>45658</v>
+      <c r="C41" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D41" t="s">
         <v>128</v>
@@ -1524,8 +1606,8 @@
       <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="2">
-        <v>45200</v>
+      <c r="C42" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="D42" t="s">
         <v>128</v>
@@ -1541,8 +1623,8 @@
       <c r="B43" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="2">
-        <v>45292</v>
+      <c r="C43" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D43" t="s">
         <v>128</v>
@@ -1558,8 +1640,8 @@
       <c r="B44" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="2">
-        <v>45809</v>
+      <c r="C44" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="D44" t="s">
         <v>128</v>
@@ -1575,8 +1657,8 @@
       <c r="B45" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="2">
-        <v>45017</v>
+      <c r="C45" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="D45" t="s">
         <v>128</v>
@@ -1592,8 +1674,8 @@
       <c r="B46" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="2">
-        <v>45566</v>
+      <c r="C46" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D46" t="s">
         <v>128</v>
@@ -1609,8 +1691,8 @@
       <c r="B47" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="2">
-        <v>45566</v>
+      <c r="C47" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D47" t="s">
         <v>128</v>
@@ -1621,13 +1703,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" t="s">
         <v>131</v>
       </c>
-      <c r="B48" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="2">
-        <v>45658</v>
+      <c r="C48" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D48" t="s">
         <v>128</v>
@@ -1643,8 +1725,8 @@
       <c r="B49" t="s">
         <v>10</v>
       </c>
-      <c r="C49" s="2">
-        <v>45352</v>
+      <c r="C49" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="D49" t="s">
         <v>128</v>
@@ -1660,8 +1742,8 @@
       <c r="B50" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="2">
-        <v>45017</v>
+      <c r="C50" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="D50" t="s">
         <v>128</v>
@@ -1677,8 +1759,8 @@
       <c r="B51" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="2">
-        <v>45139</v>
+      <c r="C51" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="D51" t="s">
         <v>128</v>
@@ -1694,8 +1776,8 @@
       <c r="B52" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="2">
-        <v>45689</v>
+      <c r="C52" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D52" t="s">
         <v>128</v>
@@ -1711,8 +1793,8 @@
       <c r="B53" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="2">
-        <v>45536</v>
+      <c r="C53" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="D53" t="s">
         <v>128</v>
@@ -1728,8 +1810,8 @@
       <c r="B54" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="2">
-        <v>45200</v>
+      <c r="C54" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="D54" t="s">
         <v>128</v>
@@ -1745,8 +1827,8 @@
       <c r="B55" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="2">
-        <v>45566</v>
+      <c r="C55" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D55" t="s">
         <v>128</v>
@@ -1762,8 +1844,8 @@
       <c r="B56" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="2">
-        <v>45352</v>
+      <c r="C56" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="D56" t="s">
         <v>128</v>
@@ -1779,8 +1861,8 @@
       <c r="B57" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="2">
-        <v>45078</v>
+      <c r="C57" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="D57" t="s">
         <v>128</v>
@@ -1796,8 +1878,8 @@
       <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="2">
-        <v>45474</v>
+      <c r="C58" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D58" t="s">
         <v>128</v>
@@ -1813,8 +1895,8 @@
       <c r="B59" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="2">
-        <v>45566</v>
+      <c r="C59" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D59" t="s">
         <v>128</v>
@@ -1830,8 +1912,8 @@
       <c r="B60" t="s">
         <v>94</v>
       </c>
-      <c r="C60" s="2">
-        <v>45352</v>
+      <c r="C60" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="D60" t="s">
         <v>128</v>
@@ -1847,8 +1929,8 @@
       <c r="B61" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="2">
-        <v>45352</v>
+      <c r="C61" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="D61" t="s">
         <v>128</v>
@@ -1864,8 +1946,8 @@
       <c r="B62" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="2">
-        <v>45383</v>
+      <c r="C62" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D62" t="s">
         <v>128</v>
@@ -1881,8 +1963,8 @@
       <c r="B63" t="s">
         <v>82</v>
       </c>
-      <c r="C63" s="2">
-        <v>45292</v>
+      <c r="C63" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D63" t="s">
         <v>128</v>
@@ -1898,8 +1980,8 @@
       <c r="B64" t="s">
         <v>82</v>
       </c>
-      <c r="C64" s="2">
-        <v>45292</v>
+      <c r="C64" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D64" t="s">
         <v>128</v>
@@ -1915,8 +1997,8 @@
       <c r="B65" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="2">
-        <v>45078</v>
+      <c r="C65" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="D65" t="s">
         <v>128</v>
@@ -1932,8 +2014,8 @@
       <c r="B66" t="s">
         <v>37</v>
       </c>
-      <c r="C66" s="2">
-        <v>45078</v>
+      <c r="C66" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="D66" t="s">
         <v>128</v>
@@ -1949,8 +2031,8 @@
       <c r="B67" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="2">
-        <v>45170</v>
+      <c r="C67" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="D67" t="s">
         <v>128</v>
@@ -1966,8 +2048,8 @@
       <c r="B68" t="s">
         <v>21</v>
       </c>
-      <c r="C68" s="2">
-        <v>45505</v>
+      <c r="C68" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="D68" t="s">
         <v>128</v>
@@ -1983,8 +2065,8 @@
       <c r="B69" t="s">
         <v>21</v>
       </c>
-      <c r="C69" s="2">
-        <v>45292</v>
+      <c r="C69" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D69" t="s">
         <v>128</v>
@@ -2000,8 +2082,8 @@
       <c r="B70" t="s">
         <v>21</v>
       </c>
-      <c r="C70" s="2">
-        <v>45505</v>
+      <c r="C70" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="D70" t="s">
         <v>128</v>
@@ -2017,8 +2099,8 @@
       <c r="B71" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="2">
-        <v>45505</v>
+      <c r="C71" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="D71" t="s">
         <v>128</v>
@@ -2034,8 +2116,8 @@
       <c r="B72" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="2">
-        <v>45292</v>
+      <c r="C72" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D72" t="s">
         <v>128</v>
@@ -2051,8 +2133,8 @@
       <c r="B73" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="2">
-        <v>45474</v>
+      <c r="C73" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D73" t="s">
         <v>128</v>
@@ -2068,8 +2150,8 @@
       <c r="B74" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="2">
-        <v>45108</v>
+      <c r="C74" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D74" t="s">
         <v>128</v>
@@ -2085,8 +2167,8 @@
       <c r="B75" t="s">
         <v>65</v>
       </c>
-      <c r="C75" s="2">
-        <v>45717</v>
+      <c r="C75" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="D75" t="s">
         <v>128</v>
@@ -2102,8 +2184,8 @@
       <c r="B76" t="s">
         <v>65</v>
       </c>
-      <c r="C76" s="2">
-        <v>45292</v>
+      <c r="C76" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D76" t="s">
         <v>128</v>
@@ -2119,8 +2201,8 @@
       <c r="B77" t="s">
         <v>65</v>
       </c>
-      <c r="C77" s="2">
-        <v>45474</v>
+      <c r="C77" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D77" t="s">
         <v>128</v>
@@ -2136,8 +2218,8 @@
       <c r="B78" t="s">
         <v>65</v>
       </c>
-      <c r="C78" s="2">
-        <v>45292</v>
+      <c r="C78" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D78" t="s">
         <v>128</v>
@@ -2153,8 +2235,8 @@
       <c r="B79" t="s">
         <v>65</v>
       </c>
-      <c r="C79" s="2">
-        <v>45474</v>
+      <c r="C79" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D79" t="s">
         <v>128</v>
@@ -2170,8 +2252,8 @@
       <c r="B80" t="s">
         <v>39</v>
       </c>
-      <c r="C80" s="2">
-        <v>44896</v>
+      <c r="C80" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="D80" t="s">
         <v>128</v>
@@ -2187,8 +2269,8 @@
       <c r="B81" t="s">
         <v>63</v>
       </c>
-      <c r="C81" s="2">
-        <v>45474</v>
+      <c r="C81" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D81" t="s">
         <v>128</v>
@@ -2204,8 +2286,8 @@
       <c r="B82" t="s">
         <v>63</v>
       </c>
-      <c r="C82" s="2">
-        <v>45474</v>
+      <c r="C82" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D82" t="s">
         <v>128</v>
@@ -2221,8 +2303,8 @@
       <c r="B83" t="s">
         <v>63</v>
       </c>
-      <c r="C83" s="2">
-        <v>45474</v>
+      <c r="C83" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D83" t="s">
         <v>128</v>
@@ -2238,8 +2320,8 @@
       <c r="B84" t="s">
         <v>63</v>
       </c>
-      <c r="C84" s="2">
-        <v>45505</v>
+      <c r="C84" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="D84" t="s">
         <v>128</v>
@@ -2255,8 +2337,8 @@
       <c r="B85" t="s">
         <v>63</v>
       </c>
-      <c r="C85" s="2">
-        <v>45505</v>
+      <c r="C85" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="D85" t="s">
         <v>128</v>
@@ -2272,8 +2354,8 @@
       <c r="B86" t="s">
         <v>63</v>
       </c>
-      <c r="C86" s="2">
-        <v>45505</v>
+      <c r="C86" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="D86" t="s">
         <v>128</v>
@@ -2289,8 +2371,8 @@
       <c r="B87" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="2">
-        <v>45748</v>
+      <c r="C87" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="D87" t="s">
         <v>128</v>
@@ -2306,8 +2388,8 @@
       <c r="B88" t="s">
         <v>80</v>
       </c>
-      <c r="C88" s="2">
-        <v>45689</v>
+      <c r="C88" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D88" t="s">
         <v>128</v>
@@ -2323,8 +2405,8 @@
       <c r="B89" t="s">
         <v>80</v>
       </c>
-      <c r="C89" s="2">
-        <v>45689</v>
+      <c r="C89" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D89" t="s">
         <v>128</v>
@@ -2340,8 +2422,8 @@
       <c r="B90" t="s">
         <v>80</v>
       </c>
-      <c r="C90" s="2">
-        <v>45292</v>
+      <c r="C90" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D90" t="s">
         <v>128</v>
@@ -2357,8 +2439,8 @@
       <c r="B91" t="s">
         <v>80</v>
       </c>
-      <c r="C91" s="2">
-        <v>45292</v>
+      <c r="C91" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D91" t="s">
         <v>128</v>
@@ -2374,8 +2456,8 @@
       <c r="B92" t="s">
         <v>80</v>
       </c>
-      <c r="C92" s="2">
-        <v>45383</v>
+      <c r="C92" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D92" t="s">
         <v>128</v>
@@ -2391,8 +2473,8 @@
       <c r="B93" t="s">
         <v>80</v>
       </c>
-      <c r="C93" s="2">
-        <v>45689</v>
+      <c r="C93" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D93" t="s">
         <v>128</v>
@@ -2408,8 +2490,8 @@
       <c r="B94" t="s">
         <v>80</v>
       </c>
-      <c r="C94" s="2">
-        <v>45689</v>
+      <c r="C94" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D94" t="s">
         <v>128</v>
@@ -2425,8 +2507,8 @@
       <c r="B95" t="s">
         <v>80</v>
       </c>
-      <c r="C95" s="2">
-        <v>45689</v>
+      <c r="C95" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D95" t="s">
         <v>128</v>
@@ -2442,8 +2524,8 @@
       <c r="B96" t="s">
         <v>80</v>
       </c>
-      <c r="C96" s="2">
-        <v>45689</v>
+      <c r="C96" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D96" t="s">
         <v>128</v>
@@ -2454,13 +2536,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B97" t="s">
         <v>80</v>
       </c>
-      <c r="C97" s="2">
-        <v>45292</v>
+      <c r="C97" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D97" t="s">
         <v>128</v>
@@ -2476,8 +2558,8 @@
       <c r="B98" t="s">
         <v>80</v>
       </c>
-      <c r="C98" s="2">
-        <v>45383</v>
+      <c r="C98" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D98" t="s">
         <v>128</v>
@@ -2493,8 +2575,8 @@
       <c r="B99" t="s">
         <v>80</v>
       </c>
-      <c r="C99" s="2">
-        <v>45292</v>
+      <c r="C99" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D99" t="s">
         <v>128</v>
@@ -2510,8 +2592,8 @@
       <c r="B100" t="s">
         <v>80</v>
       </c>
-      <c r="C100" s="2">
-        <v>45292</v>
+      <c r="C100" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D100" t="s">
         <v>128</v>
@@ -2527,8 +2609,8 @@
       <c r="B101" t="s">
         <v>80</v>
       </c>
-      <c r="C101" s="2">
-        <v>45292</v>
+      <c r="C101" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D101" t="s">
         <v>128</v>
@@ -2544,8 +2626,8 @@
       <c r="B102" t="s">
         <v>4</v>
       </c>
-      <c r="C102" s="2">
-        <v>45839</v>
+      <c r="C102" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="D102" t="s">
         <v>128</v>
@@ -2561,8 +2643,8 @@
       <c r="B103" t="s">
         <v>4</v>
       </c>
-      <c r="C103" s="2">
-        <v>45839</v>
+      <c r="C103" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="D103" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Site updated: 2025-11-10 13:59:51
</commit_message>
<xml_diff>
--- a/travel-map/截至20250806.xlsx
+++ b/travel-map/截至20250806.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myblog\source\travel-map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7596FE42-3977-4525-96F6-AB415310C603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE77E32-EA20-4734-8D2A-9E3A11686B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="160">
   <si>
     <t>time</t>
   </si>
@@ -512,6 +512,14 @@
   </si>
   <si>
     <t>2025年7月</t>
+  </si>
+  <si>
+    <t>舟山市</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>浙江省</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -888,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -2653,6 +2661,23 @@
         <v>128</v>
       </c>
     </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>158</v>
+      </c>
+      <c r="B104" t="s">
+        <v>159</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D104" t="s">
+        <v>128</v>
+      </c>
+      <c r="E104" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E112">
     <sortCondition ref="B1:B112"/>

</xml_diff>